<commit_message>
finalização de todos os componentes
</commit_message>
<xml_diff>
--- a/Docs/Instruções.xlsx
+++ b/Docs/Instruções.xlsx
@@ -336,9 +336,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -364,8 +364,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,8 +395,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -394,33 +418,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -433,7 +434,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -447,17 +463,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,28 +472,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,10 +486,25 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -523,19 +523,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,7 +583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,37 +595,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,25 +631,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,37 +649,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,31 +691,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -864,6 +864,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -879,13 +903,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -907,39 +935,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -947,8 +947,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -957,152 +957,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1136,13 +1136,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
@@ -1157,9 +1151,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1178,13 +1169,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1253,20 +1238,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1913,7 +1886,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20516215" y="1847850"/>
+          <a:off x="20659090" y="1847850"/>
           <a:ext cx="400050" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1957,7 +1930,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20915630" y="1847850"/>
+          <a:off x="21058505" y="1847850"/>
           <a:ext cx="15875" cy="2983865"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2046,7 +2019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6905625" y="5981700"/>
-          <a:ext cx="12829540" cy="0"/>
+          <a:ext cx="12972415" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2089,7 +2062,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19735165" y="3162300"/>
+          <a:off x="19878040" y="3162300"/>
           <a:ext cx="9525" cy="2819400"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2559,7 +2532,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 58763"/>
+            <a:gd name="adj1" fmla="val 43416"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2880,7 +2853,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="12071985" y="4828540"/>
-          <a:ext cx="8862695" cy="19685"/>
+          <a:ext cx="9005570" cy="19685"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3320,9 +3293,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>476885</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>95885</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -3332,7 +3305,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1057275" y="666750"/>
-          <a:ext cx="16420465" cy="57150"/>
+          <a:ext cx="16383000" cy="29210"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3402,15 +3375,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>459740</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>113030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>459740</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>128270</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -3419,8 +3392,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="17468215" y="714375"/>
-          <a:ext cx="0" cy="685800"/>
+          <a:off x="17423130" y="713105"/>
+          <a:ext cx="0" cy="701040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3739,675 +3712,675 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="49"/>
-      <c r="O2" s="38" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="44"/>
+      <c r="O2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="S2" s="50" t="s">
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="S2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="2:27">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="I3" s="33"/>
+      <c r="J3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="O3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="38"/>
-      <c r="S3" s="51" t="s">
+      <c r="Q3" s="33"/>
+      <c r="S3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="52" t="s">
+      <c r="V3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="52" t="s">
+      <c r="W3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="52" t="s">
+      <c r="X3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="52" t="s">
+      <c r="Y3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="52" t="s">
+      <c r="Z3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="52" t="s">
+      <c r="AA3" s="38" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:27">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="33">
         <v>0</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="33">
         <v>0</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="33">
         <v>0</v>
       </c>
-      <c r="K4" s="38">
+      <c r="K4" s="33">
         <v>0</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="O4" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="38">
+      <c r="P4" s="33">
         <v>0</v>
       </c>
-      <c r="Q4" s="38">
+      <c r="Q4" s="33">
         <v>0</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="54">
+      <c r="T4" s="46">
         <v>0</v>
       </c>
-      <c r="U4" s="54">
+      <c r="U4" s="46">
         <v>0.1</v>
       </c>
-      <c r="V4" s="54">
+      <c r="V4" s="46">
         <v>0</v>
       </c>
-      <c r="W4" s="54">
+      <c r="W4" s="46">
         <v>0</v>
       </c>
-      <c r="X4" s="54">
+      <c r="X4" s="46">
         <v>0</v>
       </c>
-      <c r="Y4" s="54">
+      <c r="Y4" s="46">
         <v>0</v>
       </c>
-      <c r="Z4" s="54">
+      <c r="Z4" s="46">
         <v>1</v>
       </c>
-      <c r="AA4" s="50">
+      <c r="AA4" s="33">
         <f>T4+U4+V4+W4+X4+Y4+Z4</f>
         <v>1.1</v>
       </c>
     </row>
     <row r="5" spans="2:27">
-      <c r="B5" s="41"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="33">
         <v>0</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="33">
         <v>0</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="33">
         <v>0</v>
       </c>
-      <c r="K5" s="38">
+      <c r="K5" s="33">
         <v>1</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="38">
+      <c r="P5" s="33">
         <v>0</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="33">
         <v>1</v>
       </c>
-      <c r="S5" s="53" t="s">
+      <c r="S5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54">
+      <c r="T5" s="46"/>
+      <c r="U5" s="46">
         <v>0.1</v>
       </c>
-      <c r="V5" s="54"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="50">
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="33">
         <f t="shared" ref="AA5:AA10" si="0">T5+U5+V5+W5+X5+Y5+Z5</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="2:27">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="33">
         <v>0</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="33">
         <v>0</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="33">
         <v>1</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="33">
         <v>0</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="38">
+      <c r="P6" s="33">
         <v>1</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6" s="33">
         <v>0</v>
       </c>
-      <c r="S6" s="53" t="s">
+      <c r="S6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54">
+      <c r="T6" s="46"/>
+      <c r="U6" s="46">
         <v>0.1</v>
       </c>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="54"/>
-      <c r="AA6" s="50">
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="2:27">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="O7" s="38" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="O7" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="33">
         <v>1</v>
       </c>
-      <c r="Q7" s="38">
+      <c r="Q7" s="33">
         <v>1</v>
       </c>
       <c r="R7" t="s">
         <v>36</v>
       </c>
-      <c r="S7" s="55" t="s">
+      <c r="S7" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54">
+      <c r="T7" s="46"/>
+      <c r="U7" s="46">
         <v>0.1</v>
       </c>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="50">
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="2:27">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="36" t="s">
+      <c r="E8" s="43"/>
+      <c r="F8" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="38" t="s">
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38" t="s">
+      <c r="K8" s="33"/>
+      <c r="L8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="S8" s="53" t="s">
+      <c r="S8" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54">
+      <c r="T8" s="46"/>
+      <c r="U8" s="46">
         <v>0.1</v>
       </c>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="50">
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="2:27">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="38">
         <v>0</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="38">
         <v>0</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="38">
         <v>1</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="38">
         <v>1</v>
       </c>
-      <c r="L9" s="43" t="s">
+      <c r="L9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O9" s="38" t="s">
+      <c r="O9" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="S9" s="53" t="s">
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="S9" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54">
+      <c r="T9" s="46"/>
+      <c r="U9" s="46">
         <v>0.1</v>
       </c>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
-      <c r="Z9" s="54"/>
-      <c r="AA9" s="50">
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="15:27">
-      <c r="O10" s="38" t="s">
+      <c r="O10" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="P10" s="38" t="s">
+      <c r="P10" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="Q10" s="38"/>
-      <c r="S10" s="53" t="s">
+      <c r="Q10" s="33"/>
+      <c r="S10" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="T10" s="54"/>
-      <c r="U10" s="54">
+      <c r="T10" s="46"/>
+      <c r="U10" s="46">
         <v>0.1</v>
       </c>
-      <c r="V10" s="54"/>
-      <c r="W10" s="54"/>
-      <c r="X10" s="54"/>
-      <c r="Y10" s="54"/>
-      <c r="Z10" s="54"/>
-      <c r="AA10" s="50">
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="46"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="33">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="2:17">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="49"/>
-      <c r="O11" s="38" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="44"/>
+      <c r="O11" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="38">
+      <c r="P11" s="33">
         <v>0</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:17">
-      <c r="B12" s="44"/>
-      <c r="C12" s="38" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38" t="s">
+      <c r="E12" s="33"/>
+      <c r="F12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38" t="s">
+      <c r="G12" s="33"/>
+      <c r="H12" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38" t="s">
+      <c r="I12" s="33"/>
+      <c r="J12" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38" t="s">
+      <c r="K12" s="33"/>
+      <c r="L12" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="38" t="s">
+      <c r="M12" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="38" t="s">
+      <c r="O12" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="P12" s="38">
+      <c r="P12" s="33">
         <v>0</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:17">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="33">
         <v>0</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="33">
         <v>1</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="K13" s="38" t="s">
+      <c r="K13" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="M13" s="38" t="s">
+      <c r="M13" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="O13" s="38" t="s">
+      <c r="O13" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="38">
+      <c r="P13" s="33">
         <v>1</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:17">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="33">
         <v>1</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="33">
         <v>0</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="38" t="s">
+      <c r="L14" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="38" t="s">
+      <c r="M14" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="O14" s="38" t="s">
+      <c r="O14" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="P14" s="38">
+      <c r="P14" s="33">
         <v>1</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="47"/>
-      <c r="C15" s="38" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="33">
         <v>1</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="33">
         <v>1</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J15" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="33" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="3:4">
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
     </row>
     <row r="18" spans="3:4">
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="3:10">
-      <c r="C19" s="22"/>
-      <c r="D19" s="22">
+      <c r="C19" s="19"/>
+      <c r="D19" s="19">
         <v>0</v>
       </c>
       <c r="E19">
@@ -4463,7 +4436,7 @@
   <dimension ref="C4:X32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O1" sqref="O$1:O$1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
@@ -4475,6 +4448,7 @@
     <col min="14" max="14" width="13.1111111111111" customWidth="1"/>
     <col min="15" max="15" width="6.65925925925926" customWidth="1"/>
     <col min="20" max="20" width="11.1111111111111" customWidth="1"/>
+    <col min="22" max="22" width="10.5555555555556" customWidth="1"/>
     <col min="24" max="24" width="14.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4532,28 +4506,28 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="23"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="24" t="s">
+      <c r="R6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="24" t="s">
+      <c r="V6" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
     </row>
     <row r="7" ht="18" spans="4:24">
       <c r="D7" s="2"/>
@@ -4563,7 +4537,7 @@
       <c r="H7" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="7" t="s">
         <v>67</v>
       </c>
       <c r="J7" s="1"/>
@@ -4572,11 +4546,11 @@
         <v>68</v>
       </c>
       <c r="M7" s="9"/>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="7" t="s">
         <v>69</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="31">
+      <c r="P7" s="26">
         <v>0</v>
       </c>
       <c r="Q7" s="1"/>
@@ -4584,13 +4558,13 @@
         <v>70</v>
       </c>
       <c r="S7" s="1"/>
-      <c r="T7" s="25" t="s">
+      <c r="T7" s="7" t="s">
         <v>71</v>
       </c>
       <c r="U7" s="1"/>
       <c r="V7" s="10"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="34"/>
+      <c r="X7" s="29"/>
     </row>
     <row r="8" ht="18" spans="4:24">
       <c r="D8" s="2"/>
@@ -4600,24 +4574,24 @@
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="25"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="25"/>
+      <c r="N8" s="7"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="17" t="s">
+      <c r="P8" s="15" t="s">
         <v>73</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="8"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="25"/>
+      <c r="T8" s="7"/>
       <c r="U8" s="1"/>
       <c r="V8" s="10"/>
       <c r="W8" s="2"/>
-      <c r="X8" s="34"/>
+      <c r="X8" s="29"/>
     </row>
     <row r="9" ht="18" spans="4:24">
       <c r="D9" s="2"/>
@@ -4629,7 +4603,7 @@
       <c r="H9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="7" t="s">
         <v>76</v>
       </c>
       <c r="K9" s="1"/>
@@ -4637,25 +4611,25 @@
         <v>77</v>
       </c>
       <c r="M9" s="9"/>
-      <c r="N9" s="25"/>
+      <c r="N9" s="7"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="32">
+      <c r="P9" s="27">
         <v>1</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="8"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="25" t="s">
+      <c r="T9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="U9" s="1"/>
       <c r="V9" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="W9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="X9" s="25"/>
+      <c r="X9" s="7"/>
     </row>
     <row r="10" ht="18" spans="4:24">
       <c r="D10" s="2"/>
@@ -4663,22 +4637,22 @@
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="25"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="8"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="25"/>
+      <c r="N10" s="7"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="8"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="25"/>
+      <c r="T10" s="7"/>
       <c r="U10" s="1"/>
       <c r="V10" s="8"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="25"/>
+      <c r="X10" s="7"/>
     </row>
     <row r="11" ht="18" spans="4:24">
       <c r="D11" s="2"/>
@@ -4686,14 +4660,14 @@
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="25"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
       <c r="L11" s="8" t="s">
         <v>81</v>
       </c>
       <c r="M11" s="9"/>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="7" t="s">
         <v>82</v>
       </c>
       <c r="O11" s="1"/>
@@ -4703,11 +4677,11 @@
         <v>83</v>
       </c>
       <c r="S11" s="1"/>
-      <c r="T11" s="25"/>
+      <c r="T11" s="7"/>
       <c r="U11" s="1"/>
       <c r="V11" s="8"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="25"/>
+      <c r="X11" s="7"/>
     </row>
     <row r="12" ht="18" spans="3:24">
       <c r="C12" s="3" t="s">
@@ -4720,22 +4694,22 @@
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="25"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
       <c r="L12" s="8"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="25"/>
+      <c r="N12" s="7"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="8"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="25"/>
+      <c r="T12" s="7"/>
       <c r="U12" s="1"/>
       <c r="V12" s="8"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="25"/>
+      <c r="X12" s="7"/>
     </row>
     <row r="13" ht="18" spans="4:24">
       <c r="D13" s="2"/>
@@ -4745,38 +4719,38 @@
       <c r="H13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="7" t="s">
         <v>87</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="26" t="s">
+      <c r="M13" s="13"/>
+      <c r="N13" s="22" t="s">
         <v>56</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="15" t="s">
+      <c r="R13" s="12"/>
+      <c r="S13" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="T13" s="26"/>
+      <c r="T13" s="22"/>
       <c r="U13" s="1"/>
       <c r="V13" s="8"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="25"/>
+      <c r="X13" s="7"/>
     </row>
     <row r="14" ht="18" spans="4:24">
       <c r="D14" s="1"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
-      <c r="I14" s="25"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -4789,29 +4763,29 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="33" t="s">
+      <c r="V14" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="W14" s="21"/>
-      <c r="X14" s="26" t="s">
+      <c r="W14" s="18"/>
+      <c r="X14" s="22" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" ht="18" spans="4:24">
       <c r="D15" s="1"/>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="26"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="21" t="s">
         <v>94</v>
       </c>
       <c r="N15" s="1"/>
@@ -4859,10 +4833,10 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="24" t="s">
+      <c r="N17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="24"/>
+      <c r="O17" s="21"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -4883,9 +4857,9 @@
       <c r="J18" s="9"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="22"/>
+      <c r="M18" s="19"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="25"/>
+      <c r="O18" s="7"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -4903,14 +4877,14 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="33" t="s">
+      <c r="M19" s="19"/>
+      <c r="N19" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="O19" s="30"/>
+      <c r="O19" s="25"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -4969,12 +4943,12 @@
     <row r="22" ht="18" spans="4:24">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="I22" s="28"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -4993,13 +4967,13 @@
     <row r="23" ht="18" spans="4:24">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I23" s="29"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="1"/>
@@ -5019,11 +4993,11 @@
     <row r="24" ht="18" spans="4:24">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="18" t="s">
+      <c r="G24" s="16"/>
+      <c r="H24" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I24" s="29"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="1"/>
@@ -5042,13 +5016,13 @@
     <row r="25" ht="18" spans="4:24">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="I25" s="29"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="1"/>
@@ -5068,11 +5042,11 @@
     <row r="26" ht="18" spans="4:24">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="18" t="s">
+      <c r="G26" s="16"/>
+      <c r="H26" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I26" s="29"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="1"/>
@@ -5092,11 +5066,11 @@
     <row r="27" ht="18" spans="4:24">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21" t="s">
+      <c r="G27" s="17"/>
+      <c r="H27" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="I27" s="30"/>
+      <c r="I27" s="25"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="1"/>
@@ -5121,7 +5095,7 @@
         <v>103</v>
       </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="23"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="1"/>
@@ -5142,9 +5116,9 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="1"/>

</xml_diff>